<commit_message>
add lot AJ03 to bead catalog
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B547837F-CD96-574D-944D-DF3B010C5A34}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="6600" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="2300" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -227,9 +228,6 @@
     <t>MEBFP</t>
   </si>
   <si>
-    <t>Lot AJ02</t>
-  </si>
-  <si>
     <t>MEBV510</t>
   </si>
   <si>
@@ -297,12 +295,15 @@
   </si>
   <si>
     <t>Alexa 700</t>
+  </si>
+  <si>
+    <t>Lot AJ02, AJ03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -386,6 +387,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -653,11 +657,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2974,7 +2978,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="B77" t="s">
         <v>43</v>
@@ -3009,7 +3013,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C78">
         <v>405</v>
@@ -3018,7 +3022,7 @@
         <v>47</v>
       </c>
       <c r="E78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F78" s="1">
         <v>439.03108723579822</v>
@@ -3073,16 +3077,16 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C80">
         <v>405</v>
       </c>
       <c r="D80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E80" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F80" s="1">
         <v>356.27932187382771</v>
@@ -3105,7 +3109,7 @@
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C81">
         <v>405</v>
@@ -3114,7 +3118,7 @@
         <v>54</v>
       </c>
       <c r="E81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F81" s="1">
         <v>161.4064963311495</v>
@@ -3137,16 +3141,16 @@
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82">
         <v>405</v>
       </c>
       <c r="D82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F82" s="1">
         <v>152.00296959201486</v>
@@ -3265,7 +3269,7 @@
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C86">
         <v>561</v>
@@ -3297,7 +3301,7 @@
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C87">
         <v>488</v>
@@ -3329,13 +3333,13 @@
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C88">
         <v>561</v>
       </c>
       <c r="D88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E88" t="s">
         <v>52</v>
@@ -3361,7 +3365,7 @@
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C89">
         <v>561</v>
@@ -3370,7 +3374,7 @@
         <v>54</v>
       </c>
       <c r="E89" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F89" s="1">
         <v>194.17933650418175</v>
@@ -3399,7 +3403,7 @@
         <v>561</v>
       </c>
       <c r="D90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E90" t="s">
         <v>17</v>
@@ -3457,7 +3461,7 @@
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92">
         <v>640</v>
@@ -3466,7 +3470,7 @@
         <v>60</v>
       </c>
       <c r="E92" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F92" s="1">
         <v>826.87801778556229</v>
@@ -3495,7 +3499,7 @@
         <v>640</v>
       </c>
       <c r="D93" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E93" t="s">
         <v>22</v>
@@ -3521,16 +3525,16 @@
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C94">
         <v>355</v>
       </c>
       <c r="D94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F94" s="1">
         <v>144.00513388518888</v>
@@ -3553,16 +3557,16 @@
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C95">
         <v>355</v>
       </c>
       <c r="D95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E95" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F95" s="1">
         <v>28.126664630172691</v>

</xml_diff>

<commit_message>
Split Lot AJ02, AJ03 into separate records in the bead catalog to support latest format
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jed.singer/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895EA969-F4B4-D645-8362-AD4E17CA62E4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="6600" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="2300" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="91">
   <si>
     <t>SpheroTech RCP-30-5A</t>
   </si>
@@ -227,82 +228,85 @@
     <t>MEBFP</t>
   </si>
   <si>
+    <t>MEBV510</t>
+  </si>
+  <si>
+    <t>MEBV650</t>
+  </si>
+  <si>
+    <t>MEBV711</t>
+  </si>
+  <si>
+    <t>MEBV786</t>
+  </si>
+  <si>
+    <t>MEPCY5.5</t>
+  </si>
+  <si>
+    <t>MEAlexa 700</t>
+  </si>
+  <si>
+    <t>MEBUV395</t>
+  </si>
+  <si>
+    <t>MEBUV737</t>
+  </si>
+  <si>
+    <t>BV510</t>
+  </si>
+  <si>
+    <t>BV650</t>
+  </si>
+  <si>
+    <t>BV711</t>
+  </si>
+  <si>
+    <t>BV786</t>
+  </si>
+  <si>
+    <t>ECD</t>
+  </si>
+  <si>
+    <t>PE-Cy5.5</t>
+  </si>
+  <si>
+    <t>BUV395</t>
+  </si>
+  <si>
+    <t>BUV737</t>
+  </si>
+  <si>
+    <t>PE-Cy5 488</t>
+  </si>
+  <si>
+    <t>PE-Cy5 561</t>
+  </si>
+  <si>
+    <t>670/30</t>
+  </si>
+  <si>
+    <t>780/60</t>
+  </si>
+  <si>
+    <t>740/35</t>
+  </si>
+  <si>
+    <t>379/28</t>
+  </si>
+  <si>
+    <t>Alexa 700</t>
+  </si>
+  <si>
     <t>Lot AJ02</t>
   </si>
   <si>
-    <t>MEBV510</t>
-  </si>
-  <si>
-    <t>MEBV650</t>
-  </si>
-  <si>
-    <t>MEBV711</t>
-  </si>
-  <si>
-    <t>MEBV786</t>
-  </si>
-  <si>
-    <t>MEPCY5.5</t>
-  </si>
-  <si>
-    <t>MEAlexa 700</t>
-  </si>
-  <si>
-    <t>MEBUV395</t>
-  </si>
-  <si>
-    <t>MEBUV737</t>
-  </si>
-  <si>
-    <t>BV510</t>
-  </si>
-  <si>
-    <t>BV650</t>
-  </si>
-  <si>
-    <t>BV711</t>
-  </si>
-  <si>
-    <t>BV786</t>
-  </si>
-  <si>
-    <t>ECD</t>
-  </si>
-  <si>
-    <t>PE-Cy5.5</t>
-  </si>
-  <si>
-    <t>BUV395</t>
-  </si>
-  <si>
-    <t>BUV737</t>
-  </si>
-  <si>
-    <t>PE-Cy5 488</t>
-  </si>
-  <si>
-    <t>PE-Cy5 561</t>
-  </si>
-  <si>
-    <t>670/30</t>
-  </si>
-  <si>
-    <t>780/60</t>
-  </si>
-  <si>
-    <t>740/35</t>
-  </si>
-  <si>
-    <t>379/28</t>
-  </si>
-  <si>
-    <t>Alexa 700</t>
+    <t>Lot AJ03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -386,6 +390,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -653,11 +660,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2974,7 +2981,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="B77" t="s">
         <v>43</v>
@@ -3009,7 +3016,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C78">
         <v>405</v>
@@ -3018,7 +3025,7 @@
         <v>47</v>
       </c>
       <c r="E78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F78" s="1">
         <v>439.03108723579822</v>
@@ -3073,16 +3080,16 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C80">
         <v>405</v>
       </c>
       <c r="D80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E80" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F80" s="1">
         <v>356.27932187382771</v>
@@ -3103,9 +3110,9 @@
         <v>62364.625703974802</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C81">
         <v>405</v>
@@ -3114,7 +3121,7 @@
         <v>54</v>
       </c>
       <c r="E81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F81" s="1">
         <v>161.4064963311495</v>
@@ -3135,18 +3142,18 @@
         <v>56753.374460214582</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82">
         <v>405</v>
       </c>
       <c r="D82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F82" s="1">
         <v>152.00296959201486</v>
@@ -3167,7 +3174,7 @@
         <v>56137.007707292629</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>3</v>
       </c>
@@ -3199,7 +3206,7 @@
         <v>485705.50301505951</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>56</v>
       </c>
@@ -3231,7 +3238,7 @@
         <v>55123.971224972251</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>6</v>
       </c>
@@ -3263,9 +3270,9 @@
         <v>337422.97853423643</v>
       </c>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C86">
         <v>561</v>
@@ -3295,9 +3302,9 @@
         <v>1027045.343192119</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C87">
         <v>488</v>
@@ -3327,15 +3334,15 @@
         <v>1320053.0432920777</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C88">
         <v>561</v>
       </c>
       <c r="D88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E88" t="s">
         <v>52</v>
@@ -3359,9 +3366,9 @@
         <v>13908504.214614941</v>
       </c>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C89">
         <v>561</v>
@@ -3370,7 +3377,7 @@
         <v>54</v>
       </c>
       <c r="E89" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F89" s="1">
         <v>194.17933650418175</v>
@@ -3391,7 +3398,7 @@
         <v>542552.43098020181</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>15</v>
       </c>
@@ -3399,7 +3406,7 @@
         <v>561</v>
       </c>
       <c r="D90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E90" t="s">
         <v>17</v>
@@ -3423,7 +3430,7 @@
         <v>1390593.0249165522</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>18</v>
       </c>
@@ -3455,9 +3462,9 @@
         <v>107967.65500555185</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92">
         <v>640</v>
@@ -3466,7 +3473,7 @@
         <v>60</v>
       </c>
       <c r="E92" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F92" s="1">
         <v>826.87801778556229</v>
@@ -3487,7 +3494,7 @@
         <v>1265026.5051715351</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>21</v>
       </c>
@@ -3495,7 +3502,7 @@
         <v>640</v>
       </c>
       <c r="D93" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E93" t="s">
         <v>22</v>
@@ -3519,18 +3526,18 @@
         <v>261421.46218751947</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C94">
         <v>355</v>
       </c>
       <c r="D94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F94" s="1">
         <v>144.00513388518888</v>
@@ -3551,18 +3558,18 @@
         <v>29323.395954775358</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C95">
         <v>355</v>
       </c>
       <c r="D95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E95" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F95" s="1">
         <v>28.126664630172691</v>
@@ -3580,6 +3587,617 @@
         <v>7453.3028433327572</v>
       </c>
       <c r="K95" s="1">
+        <v>29429.229169638056</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>90</v>
+      </c>
+      <c r="B96" t="s">
+        <v>43</v>
+      </c>
+      <c r="C96">
+        <v>405</v>
+      </c>
+      <c r="D96" t="s">
+        <v>44</v>
+      </c>
+      <c r="E96" t="s">
+        <v>45</v>
+      </c>
+      <c r="F96" s="3">
+        <v>152</v>
+      </c>
+      <c r="G96" s="3">
+        <v>529</v>
+      </c>
+      <c r="H96" s="3">
+        <v>2416</v>
+      </c>
+      <c r="I96" s="3">
+        <v>5899</v>
+      </c>
+      <c r="J96" s="3">
+        <v>13266</v>
+      </c>
+      <c r="K96" s="3">
+        <v>26699</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>74</v>
+      </c>
+      <c r="C97">
+        <v>405</v>
+      </c>
+      <c r="D97" t="s">
+        <v>47</v>
+      </c>
+      <c r="E97" t="s">
+        <v>66</v>
+      </c>
+      <c r="F97" s="1">
+        <v>439.03108723579822</v>
+      </c>
+      <c r="G97" s="1">
+        <v>1128.1165738811235</v>
+      </c>
+      <c r="H97" s="1">
+        <v>5250.1626972944832</v>
+      </c>
+      <c r="I97" s="1">
+        <v>13404.439382284159</v>
+      </c>
+      <c r="J97" s="1">
+        <v>32187.960560894164</v>
+      </c>
+      <c r="K97" s="1">
+        <v>66013.697333474352</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>49</v>
+      </c>
+      <c r="C98">
+        <v>405</v>
+      </c>
+      <c r="D98" t="s">
+        <v>50</v>
+      </c>
+      <c r="E98" t="s">
+        <v>51</v>
+      </c>
+      <c r="F98" s="1">
+        <v>473.48120845241425</v>
+      </c>
+      <c r="G98" s="1">
+        <v>888.89247325914778</v>
+      </c>
+      <c r="H98" s="1">
+        <v>3308.2323795700468</v>
+      </c>
+      <c r="I98" s="1">
+        <v>8096.430093766975</v>
+      </c>
+      <c r="J98" s="1">
+        <v>21927.409708467672</v>
+      </c>
+      <c r="K98" s="1">
+        <v>63543.925886697034</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>75</v>
+      </c>
+      <c r="C99">
+        <v>405</v>
+      </c>
+      <c r="D99" t="s">
+        <v>84</v>
+      </c>
+      <c r="E99" t="s">
+        <v>67</v>
+      </c>
+      <c r="F99" s="1">
+        <v>356.27932187382771</v>
+      </c>
+      <c r="G99" s="1">
+        <v>781.34482620455105</v>
+      </c>
+      <c r="H99" s="1">
+        <v>3000.9365772192568</v>
+      </c>
+      <c r="I99" s="1">
+        <v>7266.969156879848</v>
+      </c>
+      <c r="J99" s="1">
+        <v>20931.195845993956</v>
+      </c>
+      <c r="K99" s="1">
+        <v>62364.625703974802</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>76</v>
+      </c>
+      <c r="C100">
+        <v>405</v>
+      </c>
+      <c r="D100" t="s">
+        <v>54</v>
+      </c>
+      <c r="E100" t="s">
+        <v>68</v>
+      </c>
+      <c r="F100" s="1">
+        <v>161.4064963311495</v>
+      </c>
+      <c r="G100" s="1">
+        <v>706.37121865124288</v>
+      </c>
+      <c r="H100" s="1">
+        <v>2806.2561765989694</v>
+      </c>
+      <c r="I100" s="1">
+        <v>6536.3741423501024</v>
+      </c>
+      <c r="J100" s="1">
+        <v>19293.055472706204</v>
+      </c>
+      <c r="K100" s="1">
+        <v>56753.374460214582</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>77</v>
+      </c>
+      <c r="C101">
+        <v>405</v>
+      </c>
+      <c r="D101" t="s">
+        <v>85</v>
+      </c>
+      <c r="E101" t="s">
+        <v>69</v>
+      </c>
+      <c r="F101" s="1">
+        <v>152.00296959201486</v>
+      </c>
+      <c r="G101" s="1">
+        <v>706.74870229900523</v>
+      </c>
+      <c r="H101" s="1">
+        <v>2758.2310238877872</v>
+      </c>
+      <c r="I101" s="1">
+        <v>6388.9539650885108</v>
+      </c>
+      <c r="J101" s="1">
+        <v>19061.981025414228</v>
+      </c>
+      <c r="K101" s="1">
+        <v>56137.007707292629</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102">
+        <v>488</v>
+      </c>
+      <c r="D102" t="s">
+        <v>47</v>
+      </c>
+      <c r="E102" t="s">
+        <v>5</v>
+      </c>
+      <c r="F102" s="1">
+        <v>190.37469148459621</v>
+      </c>
+      <c r="G102" s="1">
+        <v>3867.786255674208</v>
+      </c>
+      <c r="H102" s="1">
+        <v>33700.918610833403</v>
+      </c>
+      <c r="I102" s="1">
+        <v>97304.301498948014</v>
+      </c>
+      <c r="J102" s="1">
+        <v>251992.15196370424</v>
+      </c>
+      <c r="K102" s="1">
+        <v>485705.50301505951</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103">
+        <v>488</v>
+      </c>
+      <c r="D103" t="s">
+        <v>57</v>
+      </c>
+      <c r="E103" t="s">
+        <v>58</v>
+      </c>
+      <c r="F103" s="1">
+        <v>98.373492455450659</v>
+      </c>
+      <c r="G103" s="1">
+        <v>606.67301182136453</v>
+      </c>
+      <c r="H103" s="1">
+        <v>2986.1555651889935</v>
+      </c>
+      <c r="I103" s="1">
+        <v>7176.0739910682232</v>
+      </c>
+      <c r="J103" s="1">
+        <v>19997.042457093306</v>
+      </c>
+      <c r="K103" s="1">
+        <v>55123.971224972251</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104">
+        <v>488</v>
+      </c>
+      <c r="D104" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104" s="1">
+        <v>202.29113376298974</v>
+      </c>
+      <c r="G104" s="1">
+        <v>3041.3914157579152</v>
+      </c>
+      <c r="H104" s="1">
+        <v>25416.732533159342</v>
+      </c>
+      <c r="I104" s="1">
+        <v>72565.671201345162</v>
+      </c>
+      <c r="J104" s="1">
+        <v>182449.44318798327</v>
+      </c>
+      <c r="K104" s="1">
+        <v>337422.97853423643</v>
+      </c>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>78</v>
+      </c>
+      <c r="C105">
+        <v>561</v>
+      </c>
+      <c r="D105" t="s">
+        <v>50</v>
+      </c>
+      <c r="E105" t="s">
+        <v>11</v>
+      </c>
+      <c r="F105" s="1">
+        <v>9.8194131263984676</v>
+      </c>
+      <c r="G105" s="1">
+        <v>6604.493123628401</v>
+      </c>
+      <c r="H105" s="1">
+        <v>61317.026926697305</v>
+      </c>
+      <c r="I105" s="1">
+        <v>183370.75879826702</v>
+      </c>
+      <c r="J105" s="1">
+        <v>492055.089919544</v>
+      </c>
+      <c r="K105" s="1">
+        <v>1027045.343192119</v>
+      </c>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>82</v>
+      </c>
+      <c r="C106">
+        <v>488</v>
+      </c>
+      <c r="D106" t="s">
+        <v>13</v>
+      </c>
+      <c r="E106" t="s">
+        <v>52</v>
+      </c>
+      <c r="F106" s="1">
+        <v>66.18703784592276</v>
+      </c>
+      <c r="G106" s="1">
+        <v>1210.7095889196451</v>
+      </c>
+      <c r="H106" s="1">
+        <v>15491.726172542774</v>
+      </c>
+      <c r="I106" s="1">
+        <v>62603.418084031873</v>
+      </c>
+      <c r="J106" s="1">
+        <v>298933.37238125486</v>
+      </c>
+      <c r="K106" s="1">
+        <v>1320053.0432920777</v>
+      </c>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>83</v>
+      </c>
+      <c r="C107">
+        <v>561</v>
+      </c>
+      <c r="D107" t="s">
+        <v>84</v>
+      </c>
+      <c r="E107" t="s">
+        <v>52</v>
+      </c>
+      <c r="F107" s="1">
+        <v>1.8286242093445937</v>
+      </c>
+      <c r="G107" s="1">
+        <v>15553.648796520212</v>
+      </c>
+      <c r="H107" s="1">
+        <v>258845.94762038183</v>
+      </c>
+      <c r="I107" s="1">
+        <v>1076513.4803304502</v>
+      </c>
+      <c r="J107" s="1">
+        <v>4391525.6994513907</v>
+      </c>
+      <c r="K107" s="1">
+        <v>13908504.214614941</v>
+      </c>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>79</v>
+      </c>
+      <c r="C108">
+        <v>561</v>
+      </c>
+      <c r="D108" t="s">
+        <v>54</v>
+      </c>
+      <c r="E108" t="s">
+        <v>70</v>
+      </c>
+      <c r="F108" s="1">
+        <v>194.17933650418175</v>
+      </c>
+      <c r="G108" s="1">
+        <v>6371.1092741035509</v>
+      </c>
+      <c r="H108" s="1">
+        <v>31258.272638840761</v>
+      </c>
+      <c r="I108" s="1">
+        <v>75288.355853438858</v>
+      </c>
+      <c r="J108" s="1">
+        <v>211044.54021726499</v>
+      </c>
+      <c r="K108" s="1">
+        <v>542552.43098020181</v>
+      </c>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109">
+        <v>561</v>
+      </c>
+      <c r="D109" t="s">
+        <v>85</v>
+      </c>
+      <c r="E109" t="s">
+        <v>17</v>
+      </c>
+      <c r="F109" s="1">
+        <v>409.08169712983124</v>
+      </c>
+      <c r="G109" s="1">
+        <v>1839.315193213268</v>
+      </c>
+      <c r="H109" s="1">
+        <v>15107.496851930342</v>
+      </c>
+      <c r="I109" s="1">
+        <v>53705.550336100336</v>
+      </c>
+      <c r="J109" s="1">
+        <v>276146.76785855967</v>
+      </c>
+      <c r="K109" s="1">
+        <v>1390593.0249165522</v>
+      </c>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110">
+        <v>640</v>
+      </c>
+      <c r="D110" t="s">
+        <v>19</v>
+      </c>
+      <c r="E110" t="s">
+        <v>20</v>
+      </c>
+      <c r="F110" s="1">
+        <v>240.51705804576588</v>
+      </c>
+      <c r="G110" s="1">
+        <v>1215.8104555821958</v>
+      </c>
+      <c r="H110" s="1">
+        <v>6248.320419876266</v>
+      </c>
+      <c r="I110" s="1">
+        <v>16368.995601462399</v>
+      </c>
+      <c r="J110" s="1">
+        <v>49562.123258682805</v>
+      </c>
+      <c r="K110" s="1">
+        <v>107967.65500555185</v>
+      </c>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>88</v>
+      </c>
+      <c r="C111">
+        <v>640</v>
+      </c>
+      <c r="D111" t="s">
+        <v>60</v>
+      </c>
+      <c r="E111" t="s">
+        <v>71</v>
+      </c>
+      <c r="F111" s="1">
+        <v>826.87801778556229</v>
+      </c>
+      <c r="G111" s="1">
+        <v>6568.6060669587732</v>
+      </c>
+      <c r="H111" s="1">
+        <v>42676.558982756753</v>
+      </c>
+      <c r="I111" s="1">
+        <v>126158.5167588528</v>
+      </c>
+      <c r="J111" s="1">
+        <v>475479.53062918095</v>
+      </c>
+      <c r="K111" s="1">
+        <v>1265026.5051715351</v>
+      </c>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112">
+        <v>640</v>
+      </c>
+      <c r="D112" t="s">
+        <v>85</v>
+      </c>
+      <c r="E112" t="s">
+        <v>22</v>
+      </c>
+      <c r="F112" s="1">
+        <v>151.9308797993595</v>
+      </c>
+      <c r="G112" s="1">
+        <v>1502.0924486896611</v>
+      </c>
+      <c r="H112" s="1">
+        <v>9422.6636597741726</v>
+      </c>
+      <c r="I112" s="1">
+        <v>27118.905505335708</v>
+      </c>
+      <c r="J112" s="1">
+        <v>100162.00163572405</v>
+      </c>
+      <c r="K112" s="1">
+        <v>261421.46218751947</v>
+      </c>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>80</v>
+      </c>
+      <c r="C113">
+        <v>355</v>
+      </c>
+      <c r="D113" t="s">
+        <v>87</v>
+      </c>
+      <c r="E113" t="s">
+        <v>72</v>
+      </c>
+      <c r="F113" s="1">
+        <v>144.00513388518888</v>
+      </c>
+      <c r="G113" s="1">
+        <v>871.14185517691828</v>
+      </c>
+      <c r="H113" s="1">
+        <v>3857.7689119907677</v>
+      </c>
+      <c r="I113" s="1">
+        <v>8428.2864016885287</v>
+      </c>
+      <c r="J113" s="1">
+        <v>16978.910841784476</v>
+      </c>
+      <c r="K113" s="1">
+        <v>29323.395954775358</v>
+      </c>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>81</v>
+      </c>
+      <c r="C114">
+        <v>355</v>
+      </c>
+      <c r="D114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E114" t="s">
+        <v>73</v>
+      </c>
+      <c r="F114" s="1">
+        <v>28.126664630172691</v>
+      </c>
+      <c r="G114" s="1">
+        <v>183.25960593669924</v>
+      </c>
+      <c r="H114" s="1">
+        <v>785.83204702247065</v>
+      </c>
+      <c r="I114" s="1">
+        <v>2025.8877346144275</v>
+      </c>
+      <c r="J114" s="1">
+        <v>7453.3028433327572</v>
+      </c>
+      <c r="K114" s="1">
         <v>29429.229169638056</v>
       </c>
     </row>

</xml_diff>

<commit_message>
unsplit URCP lots, since issue has been resolved
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jed.singer/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895EA969-F4B4-D645-8362-AD4E17CA62E4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{10388894-A04E-E946-9639-56B9583D51AD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="2300" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="90">
   <si>
     <t>SpheroTech RCP-30-5A</t>
   </si>
@@ -297,10 +297,7 @@
     <t>Alexa 700</t>
   </si>
   <si>
-    <t>Lot AJ02</t>
-  </si>
-  <si>
-    <t>Lot AJ03</t>
+    <t>Lot AJ02, AJ03</t>
   </si>
 </sst>
 </file>
@@ -661,9 +658,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N114"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
       <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
@@ -3110,7 +3107,7 @@
         <v>62364.625703974802</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>76</v>
       </c>
@@ -3142,7 +3139,7 @@
         <v>56753.374460214582</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>77</v>
       </c>
@@ -3174,7 +3171,7 @@
         <v>56137.007707292629</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>3</v>
       </c>
@@ -3206,7 +3203,7 @@
         <v>485705.50301505951</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>56</v>
       </c>
@@ -3238,7 +3235,7 @@
         <v>55123.971224972251</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>6</v>
       </c>
@@ -3270,7 +3267,7 @@
         <v>337422.97853423643</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>78</v>
       </c>
@@ -3302,7 +3299,7 @@
         <v>1027045.343192119</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>82</v>
       </c>
@@ -3334,7 +3331,7 @@
         <v>1320053.0432920777</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>83</v>
       </c>
@@ -3366,7 +3363,7 @@
         <v>13908504.214614941</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>79</v>
       </c>
@@ -3398,7 +3395,7 @@
         <v>542552.43098020181</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>15</v>
       </c>
@@ -3430,7 +3427,7 @@
         <v>1390593.0249165522</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>18</v>
       </c>
@@ -3462,7 +3459,7 @@
         <v>107967.65500555185</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>88</v>
       </c>
@@ -3494,7 +3491,7 @@
         <v>1265026.5051715351</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>21</v>
       </c>
@@ -3526,7 +3523,7 @@
         <v>261421.46218751947</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>80</v>
       </c>
@@ -3558,7 +3555,7 @@
         <v>29323.395954775358</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>81</v>
       </c>
@@ -3587,617 +3584,6 @@
         <v>7453.3028433327572</v>
       </c>
       <c r="K95" s="1">
-        <v>29429.229169638056</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>90</v>
-      </c>
-      <c r="B96" t="s">
-        <v>43</v>
-      </c>
-      <c r="C96">
-        <v>405</v>
-      </c>
-      <c r="D96" t="s">
-        <v>44</v>
-      </c>
-      <c r="E96" t="s">
-        <v>45</v>
-      </c>
-      <c r="F96" s="3">
-        <v>152</v>
-      </c>
-      <c r="G96" s="3">
-        <v>529</v>
-      </c>
-      <c r="H96" s="3">
-        <v>2416</v>
-      </c>
-      <c r="I96" s="3">
-        <v>5899</v>
-      </c>
-      <c r="J96" s="3">
-        <v>13266</v>
-      </c>
-      <c r="K96" s="3">
-        <v>26699</v>
-      </c>
-    </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
-        <v>74</v>
-      </c>
-      <c r="C97">
-        <v>405</v>
-      </c>
-      <c r="D97" t="s">
-        <v>47</v>
-      </c>
-      <c r="E97" t="s">
-        <v>66</v>
-      </c>
-      <c r="F97" s="1">
-        <v>439.03108723579822</v>
-      </c>
-      <c r="G97" s="1">
-        <v>1128.1165738811235</v>
-      </c>
-      <c r="H97" s="1">
-        <v>5250.1626972944832</v>
-      </c>
-      <c r="I97" s="1">
-        <v>13404.439382284159</v>
-      </c>
-      <c r="J97" s="1">
-        <v>32187.960560894164</v>
-      </c>
-      <c r="K97" s="1">
-        <v>66013.697333474352</v>
-      </c>
-    </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
-        <v>49</v>
-      </c>
-      <c r="C98">
-        <v>405</v>
-      </c>
-      <c r="D98" t="s">
-        <v>50</v>
-      </c>
-      <c r="E98" t="s">
-        <v>51</v>
-      </c>
-      <c r="F98" s="1">
-        <v>473.48120845241425</v>
-      </c>
-      <c r="G98" s="1">
-        <v>888.89247325914778</v>
-      </c>
-      <c r="H98" s="1">
-        <v>3308.2323795700468</v>
-      </c>
-      <c r="I98" s="1">
-        <v>8096.430093766975</v>
-      </c>
-      <c r="J98" s="1">
-        <v>21927.409708467672</v>
-      </c>
-      <c r="K98" s="1">
-        <v>63543.925886697034</v>
-      </c>
-    </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B99" t="s">
-        <v>75</v>
-      </c>
-      <c r="C99">
-        <v>405</v>
-      </c>
-      <c r="D99" t="s">
-        <v>84</v>
-      </c>
-      <c r="E99" t="s">
-        <v>67</v>
-      </c>
-      <c r="F99" s="1">
-        <v>356.27932187382771</v>
-      </c>
-      <c r="G99" s="1">
-        <v>781.34482620455105</v>
-      </c>
-      <c r="H99" s="1">
-        <v>3000.9365772192568</v>
-      </c>
-      <c r="I99" s="1">
-        <v>7266.969156879848</v>
-      </c>
-      <c r="J99" s="1">
-        <v>20931.195845993956</v>
-      </c>
-      <c r="K99" s="1">
-        <v>62364.625703974802</v>
-      </c>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B100" t="s">
-        <v>76</v>
-      </c>
-      <c r="C100">
-        <v>405</v>
-      </c>
-      <c r="D100" t="s">
-        <v>54</v>
-      </c>
-      <c r="E100" t="s">
-        <v>68</v>
-      </c>
-      <c r="F100" s="1">
-        <v>161.4064963311495</v>
-      </c>
-      <c r="G100" s="1">
-        <v>706.37121865124288</v>
-      </c>
-      <c r="H100" s="1">
-        <v>2806.2561765989694</v>
-      </c>
-      <c r="I100" s="1">
-        <v>6536.3741423501024</v>
-      </c>
-      <c r="J100" s="1">
-        <v>19293.055472706204</v>
-      </c>
-      <c r="K100" s="1">
-        <v>56753.374460214582</v>
-      </c>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
-        <v>77</v>
-      </c>
-      <c r="C101">
-        <v>405</v>
-      </c>
-      <c r="D101" t="s">
-        <v>85</v>
-      </c>
-      <c r="E101" t="s">
-        <v>69</v>
-      </c>
-      <c r="F101" s="1">
-        <v>152.00296959201486</v>
-      </c>
-      <c r="G101" s="1">
-        <v>706.74870229900523</v>
-      </c>
-      <c r="H101" s="1">
-        <v>2758.2310238877872</v>
-      </c>
-      <c r="I101" s="1">
-        <v>6388.9539650885108</v>
-      </c>
-      <c r="J101" s="1">
-        <v>19061.981025414228</v>
-      </c>
-      <c r="K101" s="1">
-        <v>56137.007707292629</v>
-      </c>
-    </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B102" t="s">
-        <v>3</v>
-      </c>
-      <c r="C102">
-        <v>488</v>
-      </c>
-      <c r="D102" t="s">
-        <v>47</v>
-      </c>
-      <c r="E102" t="s">
-        <v>5</v>
-      </c>
-      <c r="F102" s="1">
-        <v>190.37469148459621</v>
-      </c>
-      <c r="G102" s="1">
-        <v>3867.786255674208</v>
-      </c>
-      <c r="H102" s="1">
-        <v>33700.918610833403</v>
-      </c>
-      <c r="I102" s="1">
-        <v>97304.301498948014</v>
-      </c>
-      <c r="J102" s="1">
-        <v>251992.15196370424</v>
-      </c>
-      <c r="K102" s="1">
-        <v>485705.50301505951</v>
-      </c>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B103" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103">
-        <v>488</v>
-      </c>
-      <c r="D103" t="s">
-        <v>57</v>
-      </c>
-      <c r="E103" t="s">
-        <v>58</v>
-      </c>
-      <c r="F103" s="1">
-        <v>98.373492455450659</v>
-      </c>
-      <c r="G103" s="1">
-        <v>606.67301182136453</v>
-      </c>
-      <c r="H103" s="1">
-        <v>2986.1555651889935</v>
-      </c>
-      <c r="I103" s="1">
-        <v>7176.0739910682232</v>
-      </c>
-      <c r="J103" s="1">
-        <v>19997.042457093306</v>
-      </c>
-      <c r="K103" s="1">
-        <v>55123.971224972251</v>
-      </c>
-    </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B104" t="s">
-        <v>6</v>
-      </c>
-      <c r="C104">
-        <v>488</v>
-      </c>
-      <c r="D104" t="s">
-        <v>7</v>
-      </c>
-      <c r="E104" t="s">
-        <v>8</v>
-      </c>
-      <c r="F104" s="1">
-        <v>202.29113376298974</v>
-      </c>
-      <c r="G104" s="1">
-        <v>3041.3914157579152</v>
-      </c>
-      <c r="H104" s="1">
-        <v>25416.732533159342</v>
-      </c>
-      <c r="I104" s="1">
-        <v>72565.671201345162</v>
-      </c>
-      <c r="J104" s="1">
-        <v>182449.44318798327</v>
-      </c>
-      <c r="K104" s="1">
-        <v>337422.97853423643</v>
-      </c>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B105" t="s">
-        <v>78</v>
-      </c>
-      <c r="C105">
-        <v>561</v>
-      </c>
-      <c r="D105" t="s">
-        <v>50</v>
-      </c>
-      <c r="E105" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" s="1">
-        <v>9.8194131263984676</v>
-      </c>
-      <c r="G105" s="1">
-        <v>6604.493123628401</v>
-      </c>
-      <c r="H105" s="1">
-        <v>61317.026926697305</v>
-      </c>
-      <c r="I105" s="1">
-        <v>183370.75879826702</v>
-      </c>
-      <c r="J105" s="1">
-        <v>492055.089919544</v>
-      </c>
-      <c r="K105" s="1">
-        <v>1027045.343192119</v>
-      </c>
-    </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B106" t="s">
-        <v>82</v>
-      </c>
-      <c r="C106">
-        <v>488</v>
-      </c>
-      <c r="D106" t="s">
-        <v>13</v>
-      </c>
-      <c r="E106" t="s">
-        <v>52</v>
-      </c>
-      <c r="F106" s="1">
-        <v>66.18703784592276</v>
-      </c>
-      <c r="G106" s="1">
-        <v>1210.7095889196451</v>
-      </c>
-      <c r="H106" s="1">
-        <v>15491.726172542774</v>
-      </c>
-      <c r="I106" s="1">
-        <v>62603.418084031873</v>
-      </c>
-      <c r="J106" s="1">
-        <v>298933.37238125486</v>
-      </c>
-      <c r="K106" s="1">
-        <v>1320053.0432920777</v>
-      </c>
-    </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B107" t="s">
-        <v>83</v>
-      </c>
-      <c r="C107">
-        <v>561</v>
-      </c>
-      <c r="D107" t="s">
-        <v>84</v>
-      </c>
-      <c r="E107" t="s">
-        <v>52</v>
-      </c>
-      <c r="F107" s="1">
-        <v>1.8286242093445937</v>
-      </c>
-      <c r="G107" s="1">
-        <v>15553.648796520212</v>
-      </c>
-      <c r="H107" s="1">
-        <v>258845.94762038183</v>
-      </c>
-      <c r="I107" s="1">
-        <v>1076513.4803304502</v>
-      </c>
-      <c r="J107" s="1">
-        <v>4391525.6994513907</v>
-      </c>
-      <c r="K107" s="1">
-        <v>13908504.214614941</v>
-      </c>
-    </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B108" t="s">
-        <v>79</v>
-      </c>
-      <c r="C108">
-        <v>561</v>
-      </c>
-      <c r="D108" t="s">
-        <v>54</v>
-      </c>
-      <c r="E108" t="s">
-        <v>70</v>
-      </c>
-      <c r="F108" s="1">
-        <v>194.17933650418175</v>
-      </c>
-      <c r="G108" s="1">
-        <v>6371.1092741035509</v>
-      </c>
-      <c r="H108" s="1">
-        <v>31258.272638840761</v>
-      </c>
-      <c r="I108" s="1">
-        <v>75288.355853438858</v>
-      </c>
-      <c r="J108" s="1">
-        <v>211044.54021726499</v>
-      </c>
-      <c r="K108" s="1">
-        <v>542552.43098020181</v>
-      </c>
-    </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B109" t="s">
-        <v>15</v>
-      </c>
-      <c r="C109">
-        <v>561</v>
-      </c>
-      <c r="D109" t="s">
-        <v>85</v>
-      </c>
-      <c r="E109" t="s">
-        <v>17</v>
-      </c>
-      <c r="F109" s="1">
-        <v>409.08169712983124</v>
-      </c>
-      <c r="G109" s="1">
-        <v>1839.315193213268</v>
-      </c>
-      <c r="H109" s="1">
-        <v>15107.496851930342</v>
-      </c>
-      <c r="I109" s="1">
-        <v>53705.550336100336</v>
-      </c>
-      <c r="J109" s="1">
-        <v>276146.76785855967</v>
-      </c>
-      <c r="K109" s="1">
-        <v>1390593.0249165522</v>
-      </c>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B110" t="s">
-        <v>18</v>
-      </c>
-      <c r="C110">
-        <v>640</v>
-      </c>
-      <c r="D110" t="s">
-        <v>19</v>
-      </c>
-      <c r="E110" t="s">
-        <v>20</v>
-      </c>
-      <c r="F110" s="1">
-        <v>240.51705804576588</v>
-      </c>
-      <c r="G110" s="1">
-        <v>1215.8104555821958</v>
-      </c>
-      <c r="H110" s="1">
-        <v>6248.320419876266</v>
-      </c>
-      <c r="I110" s="1">
-        <v>16368.995601462399</v>
-      </c>
-      <c r="J110" s="1">
-        <v>49562.123258682805</v>
-      </c>
-      <c r="K110" s="1">
-        <v>107967.65500555185</v>
-      </c>
-    </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B111" t="s">
-        <v>88</v>
-      </c>
-      <c r="C111">
-        <v>640</v>
-      </c>
-      <c r="D111" t="s">
-        <v>60</v>
-      </c>
-      <c r="E111" t="s">
-        <v>71</v>
-      </c>
-      <c r="F111" s="1">
-        <v>826.87801778556229</v>
-      </c>
-      <c r="G111" s="1">
-        <v>6568.6060669587732</v>
-      </c>
-      <c r="H111" s="1">
-        <v>42676.558982756753</v>
-      </c>
-      <c r="I111" s="1">
-        <v>126158.5167588528</v>
-      </c>
-      <c r="J111" s="1">
-        <v>475479.53062918095</v>
-      </c>
-      <c r="K111" s="1">
-        <v>1265026.5051715351</v>
-      </c>
-    </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B112" t="s">
-        <v>21</v>
-      </c>
-      <c r="C112">
-        <v>640</v>
-      </c>
-      <c r="D112" t="s">
-        <v>85</v>
-      </c>
-      <c r="E112" t="s">
-        <v>22</v>
-      </c>
-      <c r="F112" s="1">
-        <v>151.9308797993595</v>
-      </c>
-      <c r="G112" s="1">
-        <v>1502.0924486896611</v>
-      </c>
-      <c r="H112" s="1">
-        <v>9422.6636597741726</v>
-      </c>
-      <c r="I112" s="1">
-        <v>27118.905505335708</v>
-      </c>
-      <c r="J112" s="1">
-        <v>100162.00163572405</v>
-      </c>
-      <c r="K112" s="1">
-        <v>261421.46218751947</v>
-      </c>
-    </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B113" t="s">
-        <v>80</v>
-      </c>
-      <c r="C113">
-        <v>355</v>
-      </c>
-      <c r="D113" t="s">
-        <v>87</v>
-      </c>
-      <c r="E113" t="s">
-        <v>72</v>
-      </c>
-      <c r="F113" s="1">
-        <v>144.00513388518888</v>
-      </c>
-      <c r="G113" s="1">
-        <v>871.14185517691828</v>
-      </c>
-      <c r="H113" s="1">
-        <v>3857.7689119907677</v>
-      </c>
-      <c r="I113" s="1">
-        <v>8428.2864016885287</v>
-      </c>
-      <c r="J113" s="1">
-        <v>16978.910841784476</v>
-      </c>
-      <c r="K113" s="1">
-        <v>29323.395954775358</v>
-      </c>
-    </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B114" t="s">
-        <v>81</v>
-      </c>
-      <c r="C114">
-        <v>355</v>
-      </c>
-      <c r="D114" t="s">
-        <v>86</v>
-      </c>
-      <c r="E114" t="s">
-        <v>73</v>
-      </c>
-      <c r="F114" s="1">
-        <v>28.126664630172691</v>
-      </c>
-      <c r="G114" s="1">
-        <v>183.25960593669924</v>
-      </c>
-      <c r="H114" s="1">
-        <v>785.83204702247065</v>
-      </c>
-      <c r="I114" s="1">
-        <v>2025.8877346144275</v>
-      </c>
-      <c r="J114" s="1">
-        <v>7453.3028433327572</v>
-      </c>
-      <c r="K114" s="1">
         <v>29429.229169638056</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial pass on size bead calibration
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0C1988A8-B197-E346-B104-835807C3BF7A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45184987-29EA-784E-87FF-3BA1E3580284}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="2620" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="7820" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="96">
   <si>
     <t>SpheroTech RCP-30-5A</t>
   </si>
@@ -298,12 +298,33 @@
   </si>
   <si>
     <t>Rev E/F, Lot AJ01</t>
+  </si>
+  <si>
+    <t>SpheroTech PPS-6K</t>
+  </si>
+  <si>
+    <t>6 peaks</t>
+  </si>
+  <si>
+    <t>488/10</t>
+  </si>
+  <si>
+    <t>MEPBD</t>
+  </si>
+  <si>
+    <t>Unspecified Lot</t>
+  </si>
+  <si>
+    <t>FSC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -361,13 +382,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -658,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N95"/>
+  <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3587,6 +3609,49 @@
         <v>29429.229169638056</v>
       </c>
     </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>90</v>
+      </c>
+      <c r="B97" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>94</v>
+      </c>
+      <c r="B98" t="s">
+        <v>95</v>
+      </c>
+      <c r="C98">
+        <v>488</v>
+      </c>
+      <c r="D98" t="s">
+        <v>92</v>
+      </c>
+      <c r="E98" t="s">
+        <v>93</v>
+      </c>
+      <c r="F98" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G98" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="H98" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="I98" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="J98" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="K98" s="4">
+        <v>15.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
add bead size test
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45184987-29EA-784E-87FF-3BA1E3580284}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9DCA2A-3656-7F47-BDC1-0E9D59B685AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="7820" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="5180" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,13 +309,13 @@
     <t>488/10</t>
   </si>
   <si>
-    <t>MEPBD</t>
-  </si>
-  <si>
     <t>Unspecified Lot</t>
   </si>
   <si>
     <t>FSC</t>
+  </si>
+  <si>
+    <t>EumPBD</t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -389,7 +389,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3619,10 +3619,10 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>93</v>
+      </c>
+      <c r="B98" t="s">
         <v>94</v>
-      </c>
-      <c r="B98" t="s">
-        <v>95</v>
       </c>
       <c r="C98">
         <v>488</v>
@@ -3631,7 +3631,7 @@
         <v>92</v>
       </c>
       <c r="E98" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F98" s="4">
         <v>2.2000000000000002</v>

</xml_diff>

<commit_message>
generalize unit name handling in channels, and don't assume ERF
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9DCA2A-3656-7F47-BDC1-0E9D59B685AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BABDFFB-8FF4-3E47-8944-9400C6A621B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="5180" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -315,7 +315,7 @@
     <t>FSC</t>
   </si>
   <si>
-    <t>EumPBD</t>
+    <t>Eum</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:N98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add URQP-38-6K, fixing #406
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BABDFFB-8FF4-3E47-8944-9400C6A621B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA071298-536B-1F45-93D1-EAC013BCB1B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="5180" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1480" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="103">
   <si>
     <t>SpheroTech RCP-30-5A</t>
   </si>
@@ -316,6 +316,27 @@
   </si>
   <si>
     <t>Eum</t>
+  </si>
+  <si>
+    <t>SpheroTech URQP-30-6K</t>
+  </si>
+  <si>
+    <t>MEC30</t>
+  </si>
+  <si>
+    <t>585/40</t>
+  </si>
+  <si>
+    <t>MENR</t>
+  </si>
+  <si>
+    <t>Nile Red</t>
+  </si>
+  <si>
+    <t>Coumarin 30</t>
+  </si>
+  <si>
+    <t>Rev A</t>
   </si>
 </sst>
 </file>
@@ -680,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N98"/>
+  <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3609,46 +3630,197 @@
         <v>29429.229169638056</v>
       </c>
     </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+    </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>91</v>
       </c>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>102</v>
+      </c>
+      <c r="B98" t="s">
+        <v>101</v>
+      </c>
+      <c r="C98">
+        <v>405</v>
+      </c>
+      <c r="D98" t="s">
+        <v>43</v>
+      </c>
+      <c r="E98" t="s">
+        <v>97</v>
+      </c>
+      <c r="F98" s="1">
+        <v>374.00488807417872</v>
+      </c>
+      <c r="G98" s="1">
+        <v>86271.499287657673</v>
+      </c>
+      <c r="H98" s="1">
+        <v>267570.04923346883</v>
+      </c>
+      <c r="I98" s="1">
+        <v>620570.11667349492</v>
+      </c>
+      <c r="J98" s="1">
+        <v>2922467.8873790302</v>
+      </c>
+      <c r="K98" s="1">
+        <v>11046618.846878758</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99">
+        <v>488</v>
+      </c>
+      <c r="D99" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" t="s">
+        <v>5</v>
+      </c>
+      <c r="F99" s="1">
+        <v>95.029513558965121</v>
+      </c>
+      <c r="G99" s="1">
+        <v>14036.288491164036</v>
+      </c>
+      <c r="H99" s="1">
+        <v>49898.632436982771</v>
+      </c>
+      <c r="I99" s="1">
+        <v>116568.73085430542</v>
+      </c>
+      <c r="J99" s="1">
+        <v>528154.4113937238</v>
+      </c>
+      <c r="K99" s="1">
+        <v>1418511.5124489528</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>100</v>
+      </c>
+      <c r="C100">
+        <v>488</v>
+      </c>
+      <c r="D100" t="s">
+        <v>98</v>
+      </c>
+      <c r="E100" t="s">
+        <v>99</v>
+      </c>
+      <c r="F100" s="1">
+        <v>521.99705122975354</v>
+      </c>
+      <c r="G100" s="1">
+        <v>130320.47862080015</v>
+      </c>
+      <c r="H100" s="1">
+        <v>409386.94113308587</v>
+      </c>
+      <c r="I100" s="1">
+        <v>949625.83891307411</v>
+      </c>
+      <c r="J100" s="1">
+        <v>4233501.2166174073</v>
+      </c>
+      <c r="K100" s="1">
+        <v>13305928.130556099</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101">
+        <v>635</v>
+      </c>
+      <c r="D101" t="s">
+        <v>19</v>
+      </c>
+      <c r="E101" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1">
+        <v>1164.2779775698164</v>
+      </c>
+      <c r="H101" s="1">
+        <v>6795.3912877800885</v>
+      </c>
+      <c r="I101" s="1">
+        <v>18529.889013726759</v>
+      </c>
+      <c r="J101" s="1">
+        <v>55091.921671923526</v>
+      </c>
+      <c r="K101" s="1">
+        <v>388929.21484614135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>90</v>
+      </c>
+      <c r="B103" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>93</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B104" t="s">
         <v>94</v>
       </c>
-      <c r="C98">
-        <v>488</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="C104">
+        <v>488</v>
+      </c>
+      <c r="D104" t="s">
         <v>92</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E104" t="s">
         <v>95</v>
       </c>
-      <c r="F98" s="4">
+      <c r="F104" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G98" s="4">
+      <c r="G104" s="4">
         <v>3.2</v>
       </c>
-      <c r="H98" s="4">
+      <c r="H104" s="4">
         <v>5.5</v>
       </c>
-      <c r="I98" s="4">
+      <c r="I104" s="4">
         <v>7.5</v>
       </c>
-      <c r="J98" s="4">
+      <c r="J104" s="4">
         <v>10.5</v>
       </c>
-      <c r="K98" s="4">
+      <c r="K104" s="4">
         <v>15.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added SpheroTech URCP-38-2K lot AL02
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA071298-536B-1F45-93D1-EAC013BCB1B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC704469-E515-2144-B975-CD46692C2160}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1480" windowWidth="29180" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1760" windowWidth="23420" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,9 +294,6 @@
     <t>Alexa 700</t>
   </si>
   <si>
-    <t>Lot AJ02, AJ03</t>
-  </si>
-  <si>
     <t>Rev E/F, Lot AJ01</t>
   </si>
   <si>
@@ -337,6 +334,9 @@
   </si>
   <si>
     <t>Rev A</t>
+  </si>
+  <si>
+    <t>Lot AJ02, AJ03, AL02</t>
   </si>
 </sst>
 </file>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
         <v>42</v>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B77" t="s">
         <v>42</v>
@@ -3640,10 +3640,10 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
@@ -3654,10 +3654,10 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C98">
         <v>405</v>
@@ -3666,7 +3666,7 @@
         <v>43</v>
       </c>
       <c r="E98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F98" s="1">
         <v>374.00488807417872</v>
@@ -3721,16 +3721,16 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C100">
         <v>488</v>
       </c>
       <c r="D100" t="s">
+        <v>97</v>
+      </c>
+      <c r="E100" t="s">
         <v>98</v>
-      </c>
-      <c r="E100" t="s">
-        <v>99</v>
       </c>
       <c r="F100" s="1">
         <v>521.99705122975354</v>
@@ -3783,27 +3783,27 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>89</v>
+      </c>
+      <c r="B103" t="s">
         <v>90</v>
-      </c>
-      <c r="B103" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>92</v>
+      </c>
+      <c r="B104" t="s">
         <v>93</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104">
+        <v>488</v>
+      </c>
+      <c r="D104" t="s">
+        <v>91</v>
+      </c>
+      <c r="E104" t="s">
         <v>94</v>
-      </c>
-      <c r="C104">
-        <v>488</v>
-      </c>
-      <c r="D104" t="s">
-        <v>92</v>
-      </c>
-      <c r="E104" t="s">
-        <v>95</v>
       </c>
       <c r="F104" s="4">
         <v>2.2000000000000002</v>

</xml_diff>

<commit_message>
fix URQP catalog number and add lot AL01
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC704469-E515-2144-B975-CD46692C2160}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A8792E-CA0A-AF42-949C-A362FA0D8875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1760" windowWidth="23420" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36420" yWindow="2500" windowWidth="23420" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -315,9 +315,6 @@
     <t>Eum</t>
   </si>
   <si>
-    <t>SpheroTech URQP-30-6K</t>
-  </si>
-  <si>
     <t>MEC30</t>
   </si>
   <si>
@@ -333,10 +330,13 @@
     <t>Coumarin 30</t>
   </si>
   <si>
-    <t>Rev A</t>
-  </si>
-  <si>
     <t>Lot AJ02, AJ03, AL02</t>
+  </si>
+  <si>
+    <t>SpheroTech URQP-38-6K</t>
+  </si>
+  <si>
+    <t>Rev A, Lot AL01</t>
   </si>
 </sst>
 </file>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
         <v>42</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B97" t="s">
         <v>90</v>
@@ -3654,10 +3654,10 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C98">
         <v>405</v>
@@ -3666,7 +3666,7 @@
         <v>43</v>
       </c>
       <c r="E98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F98" s="1">
         <v>374.00488807417872</v>
@@ -3721,16 +3721,16 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C100">
         <v>488</v>
       </c>
       <c r="D100" t="s">
+        <v>96</v>
+      </c>
+      <c r="E100" t="s">
         <v>97</v>
-      </c>
-      <c r="E100" t="s">
-        <v>98</v>
       </c>
       <c r="F100" s="1">
         <v>521.99705122975354</v>

</xml_diff>

<commit_message>
Add additional spherotech 38-2K lots
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A8792E-CA0A-AF42-949C-A362FA0D8875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642710FC-DD8B-394A-AF64-24F9DD928253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36420" yWindow="2500" windowWidth="23420" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="23420" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -330,13 +330,13 @@
     <t>Coumarin 30</t>
   </si>
   <si>
-    <t>Lot AJ02, AJ03, AL02</t>
-  </si>
-  <si>
     <t>SpheroTech URQP-38-6K</t>
   </si>
   <si>
     <t>Rev A, Lot AL01</t>
+  </si>
+  <si>
+    <t>Lot AJ02, AJ03, AK01, AK02, AK03, AL01, AL02, AM01</t>
   </si>
 </sst>
 </file>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B77" t="s">
         <v>42</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B97" t="s">
         <v>90</v>
@@ -3654,7 +3654,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B98" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Add another size bead option
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642710FC-DD8B-394A-AF64-24F9DD928253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8394064-E21D-494D-8482-B89B7179D580}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="23420" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36960" yWindow="1000" windowWidth="30520" windowHeight="19480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="104">
   <si>
     <t>SpheroTech RCP-30-5A</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>Lot AJ02, AJ03, AK01, AK02, AK03, AL01, AL02, AM01</t>
+  </si>
+  <si>
+    <t>ThermoFischer F13838</t>
   </si>
 </sst>
 </file>
@@ -701,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N104"/>
+  <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="J107" sqref="J107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3824,6 +3827,49 @@
         <v>15.5</v>
       </c>
     </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>103</v>
+      </c>
+      <c r="B106" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>92</v>
+      </c>
+      <c r="B107" t="s">
+        <v>93</v>
+      </c>
+      <c r="C107">
+        <v>488</v>
+      </c>
+      <c r="D107" t="s">
+        <v>91</v>
+      </c>
+      <c r="E107" t="s">
+        <v>94</v>
+      </c>
+      <c r="F107" s="4">
+        <v>1</v>
+      </c>
+      <c r="G107" s="4">
+        <v>2</v>
+      </c>
+      <c r="H107" s="4">
+        <v>4</v>
+      </c>
+      <c r="I107" s="4">
+        <v>6</v>
+      </c>
+      <c r="J107" s="4">
+        <v>10</v>
+      </c>
+      <c r="K107" s="4">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update bead catalog entries
</commit_message>
<xml_diff>
--- a/BeadCatalog.xlsx
+++ b/BeadCatalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8394064-E21D-494D-8482-B89B7179D580}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF1D9D-C3C6-D241-B325-317A15485575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36960" yWindow="1000" windowWidth="30520" windowHeight="19480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -333,13 +333,13 @@
     <t>SpheroTech URQP-38-6K</t>
   </si>
   <si>
-    <t>Rev A, Lot AL01</t>
-  </si>
-  <si>
     <t>Lot AJ02, AJ03, AK01, AK02, AK03, AL01, AL02, AM01</t>
   </si>
   <si>
     <t>ThermoFischer F13838</t>
+  </si>
+  <si>
+    <t>Rev A, Lot AL01, AM01, AN01</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="A1:N107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B77" t="s">
         <v>42</v>
@@ -3657,7 +3657,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B98" t="s">
         <v>99</v>
@@ -3829,7 +3829,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B106" t="s">
         <v>90</v>

</xml_diff>